<commit_message>
Updated Readme @ parts
</commit_message>
<xml_diff>
--- a/data/Source Data Fig.5.xlsx
+++ b/data/Source Data Fig.5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cedric\Documents\HiWi\Willmund\GitHub\ChloroplastTools\data\figure5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\burgi\Documents\Github\ChloroplastTools\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049A99B4-CE72-4BB8-8FE4-E579B8316AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC469E7-F677-4C06-B2C5-AFADDBFBC204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="21806" windowHeight="13886" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5A) Part combinations" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="46">
   <si>
     <t>Figure 5A: Characterization of part combinations</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>petB</t>
+  </si>
+  <si>
+    <t>Figure 5C: Characterizing effect of different sites of integration</t>
   </si>
 </sst>
 </file>
@@ -467,15 +470,6 @@
   <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
@@ -488,30 +482,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -526,6 +496,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -820,532 +823,532 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.61328125" customWidth="1"/>
+    <col min="1" max="1" width="21.6328125" customWidth="1"/>
     <col min="2" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.84375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.84375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.84375" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="9.84375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="25" t="s">
+    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="17" t="s">
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="21" t="s">
+      <c r="K4" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="L4" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="22" t="s">
+      <c r="M4" s="26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="26" t="s">
+    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="24"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A6" s="15" t="s">
+      <c r="G5" s="31"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="27"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="7">
         <v>1295088</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="7">
         <v>1603795</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="7">
         <v>3698544</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="7">
         <v>2087879</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="8">
         <v>2838551</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="7">
         <v>2304771.4</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="7">
         <v>972804.38895201299</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="7">
         <v>1295088</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="7">
         <v>1603795</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="7">
         <v>2087879</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="7">
         <v>2838551</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6" s="8">
         <v>3698544</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="7">
         <v>3044967</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="7">
         <v>5846788</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="7">
         <v>2992120</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="7">
         <v>4253534</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="10">
+      <c r="F7" s="8"/>
+      <c r="G7" s="7">
         <v>4034352.25</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="7">
         <v>1341404.1428379801</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="7">
         <v>2992120</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="7">
         <v>3031755.25</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="7">
         <v>3649250.5</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="7">
         <v>4651847.5</v>
       </c>
-      <c r="M7" s="11">
+      <c r="M7" s="8">
         <v>5846788</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="7">
         <v>22675339</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="7">
         <v>5571527</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="7">
         <v>7049979</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="7">
         <v>9657296</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="8">
         <v>6802883</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="7">
         <v>10351404.800000001</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="7">
         <v>7048045.6910600504</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="7">
         <v>5571527</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="7">
         <v>6802883</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="7">
         <v>7049979</v>
       </c>
-      <c r="L8" s="10">
+      <c r="L8" s="7">
         <v>9657296</v>
       </c>
-      <c r="M8" s="11">
+      <c r="M8" s="8">
         <v>22675339</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="7">
         <v>7361236</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="7">
         <v>5533346</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="7">
         <v>9540329</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="7">
         <v>9275036</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="8">
         <v>7969005</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="7">
         <v>7935790.4000000004</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="7">
         <v>1617952.2520236101</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="7">
         <v>5533346</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="7">
         <v>7361236</v>
       </c>
-      <c r="K9" s="10">
+      <c r="K9" s="7">
         <v>7969005</v>
       </c>
-      <c r="L9" s="10">
+      <c r="L9" s="7">
         <v>9275036</v>
       </c>
-      <c r="M9" s="11">
+      <c r="M9" s="8">
         <v>9540329</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A10" s="15" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="7">
         <v>11195011</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="7">
         <v>9298959</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="7">
         <v>12875676</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="7">
         <v>8683488</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="8">
         <v>9307168</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="7">
         <v>10272060.4</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="7">
         <v>1734370.05501314</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="7">
         <v>8683488</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="7">
         <v>9298959</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="7">
         <v>9307168</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L10" s="7">
         <v>11195011</v>
       </c>
-      <c r="M10" s="11">
+      <c r="M10" s="8">
         <v>12875676</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A11" s="15" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="7">
         <v>15596084</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="7">
         <v>16093212</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="7">
         <v>14300052</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="7">
         <v>14419324</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="8">
         <v>18053494</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="7">
         <v>15692433.199999999</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="7">
         <v>1525126.8273003299</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="7">
         <v>14300052</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="7">
         <v>14419324</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="7">
         <v>15596084</v>
       </c>
-      <c r="L11" s="10">
+      <c r="L11" s="7">
         <v>16093212</v>
       </c>
-      <c r="M11" s="11">
+      <c r="M11" s="8">
         <v>18053494</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A12" s="15" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="7">
         <v>35651357</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="7">
         <v>32539346</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="7">
         <v>31481474</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="7">
         <v>34793144</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="8">
         <v>33696969</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="7">
         <v>33632458</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="7">
         <v>1676971.44018003</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="7">
         <v>31481474</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="7">
         <v>32539346</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12" s="7">
         <v>33696969</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12" s="7">
         <v>34793144</v>
       </c>
-      <c r="M12" s="11">
+      <c r="M12" s="8">
         <v>35651357</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A13" s="15" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="7">
         <v>111177464</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="7">
         <v>165856171</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="7">
         <v>109021110</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="7">
         <v>113764094</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="8">
         <v>134972564</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="7">
         <v>126958280.59999999</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="7">
         <v>24094280.637310401</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="7">
         <v>109021110</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="7">
         <v>111177464</v>
       </c>
-      <c r="K13" s="10">
+      <c r="K13" s="7">
         <v>113764094</v>
       </c>
-      <c r="L13" s="10">
+      <c r="L13" s="7">
         <v>134972564</v>
       </c>
-      <c r="M13" s="11">
+      <c r="M13" s="8">
         <v>165856171</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A14" s="15" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="7">
         <v>298819333</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="7">
         <v>138955954</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="7">
         <v>170667102</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="7">
         <v>130979522</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="8">
         <v>250638370</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="7">
         <v>198012056.19999999</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14" s="7">
         <v>73587305.849139094</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="7">
         <v>130979522</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="7">
         <v>138955954</v>
       </c>
-      <c r="K14" s="10">
+      <c r="K14" s="7">
         <v>170667102</v>
       </c>
-      <c r="L14" s="10">
+      <c r="L14" s="7">
         <v>250638370</v>
       </c>
-      <c r="M14" s="11">
+      <c r="M14" s="8">
         <v>298819333</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A15" s="15" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="7">
         <v>190902783</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="7">
         <v>198535982</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="7">
         <v>343580580</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="7">
         <v>136686757</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="8">
         <v>324319837</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="7">
         <v>238805187.80000001</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15" s="7">
         <v>90325883.982531607</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="7">
         <v>136686757</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="7">
         <v>190902783</v>
       </c>
-      <c r="K15" s="10">
+      <c r="K15" s="7">
         <v>198535982</v>
       </c>
-      <c r="L15" s="10">
+      <c r="L15" s="7">
         <v>324319837</v>
       </c>
-      <c r="M15" s="11">
+      <c r="M15" s="8">
         <v>343580580</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="16" t="s">
+    <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="10">
         <v>926093521</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="10">
         <v>910165603</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="10">
         <v>794546247</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="10">
         <v>962005944</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="11">
         <v>876058135</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="10">
         <v>893773890</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16" s="10">
         <v>63499671.4689629</v>
       </c>
-      <c r="I16" s="13">
+      <c r="I16" s="10">
         <v>794546247</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16" s="10">
         <v>876058135</v>
       </c>
-      <c r="K16" s="13">
+      <c r="K16" s="10">
         <v>910165603</v>
       </c>
-      <c r="L16" s="13">
+      <c r="L16" s="10">
         <v>926093521</v>
       </c>
-      <c r="M16" s="14">
+      <c r="M16" s="11">
         <v>962005944</v>
       </c>
     </row>
@@ -1370,453 +1373,453 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.53515625" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="25" t="s">
+    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="19" t="s">
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="21" t="s">
+      <c r="K4" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="L4" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="22" t="s">
+      <c r="M4" s="26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="26" t="s">
+    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="24"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A6" s="15" t="s">
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="27"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="6">
         <v>64288</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="7">
         <v>59541</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="7">
         <v>75847</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="7">
         <v>72336</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="8">
         <v>63413</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="7">
         <v>67085</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="7">
         <v>6755.8192323359199</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="7">
         <v>59541</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="7">
         <v>63413</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="7">
         <v>64288</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="7">
         <v>72336</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6" s="8">
         <v>75847</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="6">
         <v>1108564</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="7">
         <v>2029473</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="7">
         <v>881838</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="7">
         <v>990918</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="8">
         <v>897179</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="7">
         <v>1181594.3999999999</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="7">
         <v>482528.51425516797</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="7">
         <v>881838</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="7">
         <v>897179</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="7">
         <v>990918</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="7">
         <v>1108564</v>
       </c>
-      <c r="M7" s="11">
+      <c r="M7" s="8">
         <v>2029473</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A8" s="34" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="30">
+      <c r="B8" s="19">
         <v>5978575</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="20">
         <v>2656193</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="20">
         <v>3133686</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="20">
         <v>2358987</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="21">
         <v>1542835</v>
       </c>
-      <c r="G8" s="31">
+      <c r="G8" s="20">
         <v>3134055.2</v>
       </c>
-      <c r="H8" s="31">
+      <c r="H8" s="20">
         <v>1692066.61738159</v>
       </c>
-      <c r="I8" s="31">
+      <c r="I8" s="20">
         <v>1542835</v>
       </c>
-      <c r="J8" s="31">
+      <c r="J8" s="20">
         <v>2358987</v>
       </c>
-      <c r="K8" s="31">
+      <c r="K8" s="20">
         <v>2656193</v>
       </c>
-      <c r="L8" s="31">
+      <c r="L8" s="20">
         <v>3133686</v>
       </c>
-      <c r="M8" s="32">
+      <c r="M8" s="21">
         <v>5978575</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A9" s="33" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="16">
         <v>401892</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="17">
         <v>289013</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="17">
         <v>308205</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="17">
         <v>312053</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="18">
         <v>276040</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="17">
         <v>317440.59999999998</v>
       </c>
-      <c r="H9" s="28">
+      <c r="H9" s="17">
         <v>49417.860195479901</v>
       </c>
-      <c r="I9" s="28">
+      <c r="I9" s="17">
         <v>276040</v>
       </c>
-      <c r="J9" s="28">
+      <c r="J9" s="17">
         <v>289013</v>
       </c>
-      <c r="K9" s="28">
+      <c r="K9" s="17">
         <v>308205</v>
       </c>
-      <c r="L9" s="28">
+      <c r="L9" s="17">
         <v>312053</v>
       </c>
-      <c r="M9" s="29">
+      <c r="M9" s="18">
         <v>401892</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A10" s="15" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="6">
         <v>4706106</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="7">
         <v>4192988</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="7">
         <v>3755638</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="7">
         <v>4077091</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="8">
         <v>4201543</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="7">
         <v>4186673.2</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="7">
         <v>342005.491024193</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="7">
         <v>3755638</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="7">
         <v>4077091</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="7">
         <v>4192988</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L10" s="7">
         <v>4201543</v>
       </c>
-      <c r="M10" s="11">
+      <c r="M10" s="8">
         <v>4706106</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A11" s="34" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="30">
+      <c r="B11" s="19">
         <v>11421198</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="20">
         <v>9102085</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="20">
         <v>8421122</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E11" s="20">
         <v>9247055</v>
       </c>
-      <c r="F11" s="32">
+      <c r="F11" s="21">
         <v>8366786</v>
       </c>
-      <c r="G11" s="31">
+      <c r="G11" s="20">
         <v>9311649.1999999993</v>
       </c>
-      <c r="H11" s="31">
+      <c r="H11" s="20">
         <v>1243391.61819906</v>
       </c>
-      <c r="I11" s="31">
+      <c r="I11" s="20">
         <v>8366786</v>
       </c>
-      <c r="J11" s="31">
+      <c r="J11" s="20">
         <v>8421122</v>
       </c>
-      <c r="K11" s="31">
+      <c r="K11" s="20">
         <v>9102085</v>
       </c>
-      <c r="L11" s="31">
+      <c r="L11" s="20">
         <v>9247055</v>
       </c>
-      <c r="M11" s="32">
+      <c r="M11" s="21">
         <v>11421198</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A12" s="15" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="6">
         <v>5978575</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="7">
         <v>2656193</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="7">
         <v>3133686</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="7">
         <v>2358987</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="8">
         <v>1542835</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="7">
         <v>3134055.2</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="7">
         <v>1692066.61738159</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="7">
         <v>1542835</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="7">
         <v>2358987</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12" s="7">
         <v>2656193</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12" s="7">
         <v>3133686</v>
       </c>
-      <c r="M12" s="11">
+      <c r="M12" s="8">
         <v>5978575</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A13" s="15" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="6">
         <v>28714829</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="7">
         <v>9171482</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="7">
         <v>38762891</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="7">
         <v>8907961</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="8">
         <v>8275002</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="7">
         <v>18766433</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="7">
         <v>14125788.427673001</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="7">
         <v>8275002</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="7">
         <v>8907961</v>
       </c>
-      <c r="K13" s="10">
+      <c r="K13" s="7">
         <v>9171482</v>
       </c>
-      <c r="L13" s="10">
+      <c r="L13" s="7">
         <v>28714829</v>
       </c>
-      <c r="M13" s="11">
+      <c r="M13" s="8">
         <v>38762891</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="16" t="s">
+    <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="9">
         <v>45403389</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="10">
         <v>44263588</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="10">
         <v>46631494</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="10">
         <v>50731709</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="11">
         <v>47311907</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="10">
         <v>46868417.399999999</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="10">
         <v>2455060.1889422699</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="10">
         <v>44263588</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="10">
         <v>45403389</v>
       </c>
-      <c r="K14" s="13">
+      <c r="K14" s="10">
         <v>46631494</v>
       </c>
-      <c r="L14" s="13">
+      <c r="L14" s="10">
         <v>47311907</v>
       </c>
-      <c r="M14" s="14">
+      <c r="M14" s="11">
         <v>50731709</v>
       </c>
     </row>
-    <row r="18" spans="6:8" x14ac:dyDescent="0.4">
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
+    <row r="18" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1837,770 +1840,770 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5C95ADC-949E-4900-8EF2-28FC701941B0}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="20.765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="19" t="s">
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="21" t="s">
+      <c r="K4" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="L4" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="21" t="s">
+      <c r="M4" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="N4" s="22" t="s">
+      <c r="N4" s="26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="18"/>
-      <c r="B5" s="26" t="s">
+    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="31"/>
+      <c r="B5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="24"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="27"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="6">
         <v>39108533</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="7">
         <v>38340126</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="7">
         <v>49569084</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="7">
         <v>47797196</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="8">
         <v>40673855</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="7">
         <v>43097758.799999997</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="7">
         <v>5205455.3550956203</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="7">
         <v>38340126</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="7">
         <v>39108533</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="7">
         <v>40673855</v>
       </c>
-      <c r="M6" s="10">
+      <c r="M6" s="7">
         <v>47797196</v>
       </c>
-      <c r="N6" s="11">
+      <c r="N6" s="8">
         <v>49569084</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="36"/>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="6">
         <v>79697330</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="7">
         <v>78040257</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="7">
         <v>88188285</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="7">
         <v>105004098</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="8">
         <v>69872803</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="7">
         <v>84160554.599999994</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="7">
         <v>13343483.203128399</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="7">
         <v>69872803</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="7">
         <v>78040257</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="7">
         <v>79697330</v>
       </c>
-      <c r="M7" s="10">
+      <c r="M7" s="7">
         <v>88188285</v>
       </c>
-      <c r="N7" s="11">
+      <c r="N7" s="8">
         <v>105004098</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="36"/>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="6">
         <v>558899415</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="7">
         <v>563993574</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="7">
         <v>602434480</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="7">
         <v>603094164</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="8">
         <v>576962922</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="7">
         <v>581076911</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="7">
         <v>20865712.428727798</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="7">
         <v>558899415</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="7">
         <v>563993574</v>
       </c>
-      <c r="L8" s="10">
+      <c r="L8" s="7">
         <v>576962922</v>
       </c>
-      <c r="M8" s="10">
+      <c r="M8" s="7">
         <v>602434480</v>
       </c>
-      <c r="N8" s="11">
+      <c r="N8" s="8">
         <v>603094164</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="37"/>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="19">
         <v>840091426</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="20">
         <v>851628508</v>
       </c>
-      <c r="E9" s="31">
+      <c r="E9" s="20">
         <v>798078247</v>
       </c>
-      <c r="F9" s="31">
+      <c r="F9" s="20">
         <v>801233422</v>
       </c>
-      <c r="G9" s="32">
+      <c r="G9" s="21">
         <v>775756582</v>
       </c>
-      <c r="H9" s="31">
+      <c r="H9" s="20">
         <v>813357637</v>
       </c>
-      <c r="I9" s="31">
+      <c r="I9" s="20">
         <v>31518449.8613372</v>
       </c>
-      <c r="J9" s="31">
+      <c r="J9" s="20">
         <v>775756582</v>
       </c>
-      <c r="K9" s="31">
+      <c r="K9" s="20">
         <v>798078247</v>
       </c>
-      <c r="L9" s="31">
+      <c r="L9" s="20">
         <v>801233422</v>
       </c>
-      <c r="M9" s="31">
+      <c r="M9" s="20">
         <v>840091426</v>
       </c>
-      <c r="N9" s="32">
+      <c r="N9" s="21">
         <v>851628508</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="16">
         <v>47154729</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="17">
         <v>42189513</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="17">
         <v>49970625</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="17">
         <v>49840154</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="18">
         <v>59507583</v>
       </c>
-      <c r="H10" s="28">
+      <c r="H10" s="17">
         <v>49732520.799999997</v>
       </c>
-      <c r="I10" s="28">
+      <c r="I10" s="17">
         <v>6307973.0651905201</v>
       </c>
-      <c r="J10" s="28">
+      <c r="J10" s="17">
         <v>42189513</v>
       </c>
-      <c r="K10" s="28">
+      <c r="K10" s="17">
         <v>47154729</v>
       </c>
-      <c r="L10" s="28">
+      <c r="L10" s="17">
         <v>49840154</v>
       </c>
-      <c r="M10" s="28">
+      <c r="M10" s="17">
         <v>49970625</v>
       </c>
-      <c r="N10" s="29">
+      <c r="N10" s="18">
         <v>59507583</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="36"/>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="6">
         <v>28326631</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="7">
         <v>31888010</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="7">
         <v>26029788</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="7">
         <v>26428084</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="8">
         <v>25161972</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="7">
         <v>27566897</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="7">
         <v>2678267.94271969</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="7">
         <v>25161972</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="7">
         <v>26029788</v>
       </c>
-      <c r="L11" s="10">
+      <c r="L11" s="7">
         <v>26428084</v>
       </c>
-      <c r="M11" s="10">
+      <c r="M11" s="7">
         <v>28326631</v>
       </c>
-      <c r="N11" s="11">
+      <c r="N11" s="8">
         <v>31888010</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="36"/>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="6">
         <v>357428514</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="7">
         <v>406659915</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="7">
         <v>346617911</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="7">
         <v>402097292</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="8">
         <v>362343222</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="7">
         <v>375029370.80000001</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="7">
         <v>27436760.303989999</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="7">
         <v>346617911</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12" s="7">
         <v>357428514</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12" s="7">
         <v>362343222</v>
       </c>
-      <c r="M12" s="10">
+      <c r="M12" s="7">
         <v>402097292</v>
       </c>
-      <c r="N12" s="11">
+      <c r="N12" s="8">
         <v>406659915</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="37"/>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="30">
+      <c r="C13" s="19">
         <v>844585598</v>
       </c>
-      <c r="D13" s="31">
+      <c r="D13" s="20">
         <v>788986516</v>
       </c>
-      <c r="E13" s="31">
+      <c r="E13" s="20">
         <v>882359207</v>
       </c>
-      <c r="F13" s="31">
+      <c r="F13" s="20">
         <v>802097295</v>
       </c>
-      <c r="G13" s="32">
+      <c r="G13" s="21">
         <v>880514997</v>
       </c>
-      <c r="H13" s="31">
+      <c r="H13" s="20">
         <v>839708722.60000002</v>
       </c>
-      <c r="I13" s="31">
+      <c r="I13" s="20">
         <v>43287877.899340898</v>
       </c>
-      <c r="J13" s="31">
+      <c r="J13" s="20">
         <v>788986516</v>
       </c>
-      <c r="K13" s="31">
+      <c r="K13" s="20">
         <v>802097295</v>
       </c>
-      <c r="L13" s="31">
+      <c r="L13" s="20">
         <v>844585598</v>
       </c>
-      <c r="M13" s="31">
+      <c r="M13" s="20">
         <v>880514997</v>
       </c>
-      <c r="N13" s="32">
+      <c r="N13" s="21">
         <v>882359207</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="16">
         <v>41087061</v>
       </c>
-      <c r="D14" s="28">
+      <c r="D14" s="17">
         <v>30011964</v>
       </c>
-      <c r="E14" s="28">
+      <c r="E14" s="17">
         <v>30998370</v>
       </c>
-      <c r="F14" s="28">
+      <c r="F14" s="17">
         <v>30126233</v>
       </c>
-      <c r="G14" s="29">
+      <c r="G14" s="18">
         <v>35168167</v>
       </c>
-      <c r="H14" s="28">
+      <c r="H14" s="17">
         <v>33478359</v>
       </c>
-      <c r="I14" s="28">
+      <c r="I14" s="17">
         <v>4747388.3783004796</v>
       </c>
-      <c r="J14" s="28">
+      <c r="J14" s="17">
         <v>30011964</v>
       </c>
-      <c r="K14" s="28">
+      <c r="K14" s="17">
         <v>30126233</v>
       </c>
-      <c r="L14" s="28">
+      <c r="L14" s="17">
         <v>30998370</v>
       </c>
-      <c r="M14" s="28">
+      <c r="M14" s="17">
         <v>35168167</v>
       </c>
-      <c r="N14" s="29">
+      <c r="N14" s="18">
         <v>41087061</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="36"/>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="6">
         <v>34177522</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="7">
         <v>45976895</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="7">
         <v>35212724</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="7">
         <v>57596230</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="8">
         <v>76769320</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15" s="7">
         <v>49946538.200000003</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="7">
         <v>17744609.238136798</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="7">
         <v>34177522</v>
       </c>
-      <c r="K15" s="10">
+      <c r="K15" s="7">
         <v>35212724</v>
       </c>
-      <c r="L15" s="10">
+      <c r="L15" s="7">
         <v>45976895</v>
       </c>
-      <c r="M15" s="10">
+      <c r="M15" s="7">
         <v>57596230</v>
       </c>
-      <c r="N15" s="11">
+      <c r="N15" s="8">
         <v>76769320</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="36"/>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="6">
         <v>23219854</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="7">
         <v>22619812</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="7">
         <v>23069987</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="7">
         <v>23424868</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="8">
         <v>21948378</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="7">
         <v>22856579.800000001</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="7">
         <v>587654.60865562805</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="7">
         <v>21948378</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K16" s="7">
         <v>22619812</v>
       </c>
-      <c r="L16" s="10">
+      <c r="L16" s="7">
         <v>23069987</v>
       </c>
-      <c r="M16" s="10">
+      <c r="M16" s="7">
         <v>23219854</v>
       </c>
-      <c r="N16" s="11">
+      <c r="N16" s="8">
         <v>23424868</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="37"/>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="30">
+      <c r="C17" s="19">
         <v>240616307</v>
       </c>
-      <c r="D17" s="31">
+      <c r="D17" s="20">
         <v>162562350</v>
       </c>
-      <c r="E17" s="31">
+      <c r="E17" s="20">
         <v>169529664</v>
       </c>
-      <c r="F17" s="31">
+      <c r="F17" s="20">
         <v>133768931</v>
       </c>
-      <c r="G17" s="32">
+      <c r="G17" s="21">
         <v>235222203</v>
       </c>
-      <c r="H17" s="31">
+      <c r="H17" s="20">
         <v>188339891</v>
       </c>
-      <c r="I17" s="31">
+      <c r="I17" s="20">
         <v>47241588.625357904</v>
       </c>
-      <c r="J17" s="31">
+      <c r="J17" s="20">
         <v>133768931</v>
       </c>
-      <c r="K17" s="31">
+      <c r="K17" s="20">
         <v>162562350</v>
       </c>
-      <c r="L17" s="31">
+      <c r="L17" s="20">
         <v>169529664</v>
       </c>
-      <c r="M17" s="31">
+      <c r="M17" s="20">
         <v>235222203</v>
       </c>
-      <c r="N17" s="32">
+      <c r="N17" s="21">
         <v>240616307</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="6">
         <v>23289858</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="7">
         <v>26478237</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="7">
         <v>23886242</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="7">
         <v>71848826</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="8">
         <v>27190658</v>
       </c>
-      <c r="H18" s="10">
+      <c r="H18" s="7">
         <v>34538764.200000003</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="7">
         <v>20922604.9699011</v>
       </c>
-      <c r="J18" s="10">
+      <c r="J18" s="7">
         <v>23289858</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K18" s="7">
         <v>23886242</v>
       </c>
-      <c r="L18" s="10">
+      <c r="L18" s="7">
         <v>26478237</v>
       </c>
-      <c r="M18" s="10">
+      <c r="M18" s="7">
         <v>27190658</v>
       </c>
-      <c r="N18" s="11">
+      <c r="N18" s="8">
         <v>71848826</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="36"/>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="6">
         <v>38068789</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="7">
         <v>39233786</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="7">
         <v>38495733</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="7">
         <v>39974338</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="8">
         <v>38281182</v>
       </c>
-      <c r="H19" s="10">
+      <c r="H19" s="7">
         <v>38810765.600000001</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="7">
         <v>784710.23191003397</v>
       </c>
-      <c r="J19" s="10">
+      <c r="J19" s="7">
         <v>38068789</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K19" s="7">
         <v>38281182</v>
       </c>
-      <c r="L19" s="10">
+      <c r="L19" s="7">
         <v>38495733</v>
       </c>
-      <c r="M19" s="10">
+      <c r="M19" s="7">
         <v>39233786</v>
       </c>
-      <c r="N19" s="11">
+      <c r="N19" s="8">
         <v>39974338</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="36"/>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="6">
         <v>602049577</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="7">
         <v>575546874</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="7">
         <v>573751063</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="7">
         <v>576063301</v>
       </c>
-      <c r="G20" s="11">
+      <c r="G20" s="8">
         <v>624388229</v>
       </c>
-      <c r="H20" s="10">
+      <c r="H20" s="7">
         <v>590359808.79999995</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20" s="7">
         <v>22328500.126469601</v>
       </c>
-      <c r="J20" s="10">
+      <c r="J20" s="7">
         <v>573751063</v>
       </c>
-      <c r="K20" s="10">
+      <c r="K20" s="7">
         <v>575546874</v>
       </c>
-      <c r="L20" s="10">
+      <c r="L20" s="7">
         <v>576063301</v>
       </c>
-      <c r="M20" s="10">
+      <c r="M20" s="7">
         <v>602049577</v>
       </c>
-      <c r="N20" s="11">
+      <c r="N20" s="8">
         <v>624388229</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="38"/>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="9">
         <v>345054412</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="10">
         <v>332484794</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="10">
         <v>366841098</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="10">
         <v>427713724</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="11">
         <v>375221604</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="10">
         <v>369463126.39999998</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="10">
         <v>36729925.209911898</v>
       </c>
-      <c r="J21" s="13">
+      <c r="J21" s="10">
         <v>332484794</v>
       </c>
-      <c r="K21" s="13">
+      <c r="K21" s="10">
         <v>345054412</v>
       </c>
-      <c r="L21" s="13">
+      <c r="L21" s="10">
         <v>366841098</v>
       </c>
-      <c r="M21" s="13">
+      <c r="M21" s="10">
         <v>375221604</v>
       </c>
-      <c r="N21" s="14">
+      <c r="N21" s="11">
         <v>427713724</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>